<commit_message>
excel and properties file
</commit_message>
<xml_diff>
--- a/src/main/resources/demo.xlsx
+++ b/src/main/resources/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\weekly-classes\automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1263651F-6A74-4E21-A158-9190A239DDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B69EE28-6F19-45AF-B38A-4B84376DFC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{254F9B19-A8FE-4BFF-A95B-D05EF04AFD19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>EmpID</t>
   </si>
@@ -82,16 +82,60 @@
   </si>
   <si>
     <t>123A900</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>UAT</t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>king@123</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,15 +158,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,243 +481,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A090CBA-78B3-477A-9D08-F44C665CEA9D}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="16384" width="9.06640625" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>1001</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>10000</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>5000</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>2000</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>5000</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <f>C2+D2+E2</f>
         <v>17000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
         <f>G2-F2</f>
         <v>12000</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>44724</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>1002</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>15000</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>6000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>3000</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>4500</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
         <f t="shared" ref="G3:G6" si="0">C3+D3+E3</f>
         <v>24000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <f t="shared" ref="H3:H6" si="1">G3-F3</f>
         <v>19500</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>44724</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>1003</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>20000</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>10000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>15000</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>500</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>45000</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
         <f t="shared" si="1"/>
         <v>44500</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>44724</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>1004</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>17000</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>8000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>8000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>3000</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>33000</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>30000</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>44724</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>1005</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>12000</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>4000</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>5000</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>4000</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>21000</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>44724</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C7" s="1">
-        <f>SUM(C2:C6)</f>
+      <c r="C7">
+        <f t="shared" ref="C7:H7" si="2">SUM(C2:C6)</f>
         <v>74000</v>
       </c>
-      <c r="D7" s="1">
-        <f>SUM(D2:D6)</f>
+      <c r="D7">
+        <f t="shared" si="2"/>
         <v>33000</v>
       </c>
-      <c r="E7" s="1">
-        <f>SUM(E2:E6)</f>
+      <c r="E7">
+        <f t="shared" si="2"/>
         <v>33000</v>
       </c>
-      <c r="F7" s="1">
-        <f>SUM(F2:F6)</f>
+      <c r="F7">
+        <f t="shared" si="2"/>
         <v>17000</v>
       </c>
-      <c r="G7" s="1">
-        <f>SUM(G2:G6)</f>
+      <c r="G7">
+        <f t="shared" si="2"/>
         <v>140000</v>
       </c>
-      <c r="H7" s="1">
-        <f>SUM(H2:H6)</f>
+      <c r="H7">
+        <f t="shared" si="2"/>
         <v>123000</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>44724</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{75364BF7-E184-4ADF-88F9-0EEB6EB38B75}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{8D443AE3-89F0-4A5D-9FE1-1B8C86AB73F5}"/>
+    <hyperlink ref="D11" r:id="rId3" xr:uid="{66BE1867-FAE5-45E4-8F2D-5ECB1BC82A53}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>